<commit_message>
math, random, debugger and regex
</commit_message>
<xml_diff>
--- a/12_PDF_and_Spreadsheet/test_spreadsheet.xlsx
+++ b/12_PDF_and_Spreadsheet/test_spreadsheet.xlsx
@@ -4,10 +4,11 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
@@ -70,7 +71,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -453,72 +457,124 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="11.52" customWidth="1" style="2" min="3" max="3"/>
+    <col width="11.52" customWidth="1" style="3" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="3">
-      <c r="A1" s="2" t="n">
+    <row r="1" ht="15" customHeight="1" s="4">
+      <c r="A1" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>vik</t>
         </is>
       </c>
-      <c r="C1" s="4" t="n">
+      <c r="C1" s="5" t="n">
         <v>29874</v>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1" s="3">
-      <c r="A2" s="2" t="n">
+    <row r="2" ht="15" customHeight="1" s="4">
+      <c r="A2" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>neli</t>
         </is>
       </c>
-      <c r="C2" s="4" t="n">
+      <c r="C2" s="5" t="n">
         <v>32417</v>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" s="3">
-      <c r="A3" s="2" t="n">
+    <row r="3" ht="15" customHeight="1" s="4">
+      <c r="A3" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>victoria</t>
         </is>
       </c>
-      <c r="C3" s="4" t="n">
+      <c r="C3" s="5" t="n">
         <v>43508</v>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1" s="3">
-      <c r="A4" s="2" t="n">
+    <row r="4" ht="15" customHeight="1" s="4">
+      <c r="A4" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="inlineStr">
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>Jim</t>
         </is>
       </c>
-      <c r="C4" s="4" t="n">
+      <c r="C4" s="5" t="n">
         <v>38161</v>
       </c>
+    </row>
+    <row r="5" ht="13.8" customHeight="1" s="4">
+      <c r="D5" s="3" t="inlineStr"/>
+    </row>
+    <row r="6" ht="13.8" customHeight="1" s="4">
+      <c r="C6" s="3" t="inlineStr"/>
+    </row>
+    <row r="7" ht="15" customHeight="1" s="4">
+      <c r="B7" s="3" t="inlineStr"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetData>
+    <row r="1" ht="13.8" customHeight="1" s="4">
+      <c r="B1" s="3" t="inlineStr"/>
+    </row>
+    <row r="2"/>
+    <row r="3" ht="13.8" customHeight="1" s="4">
+      <c r="A3" s="3" t="inlineStr"/>
+    </row>
+    <row r="4" ht="13.8" customHeight="1" s="4">
+      <c r="C4" s="3" t="inlineStr"/>
+    </row>
+    <row r="5"/>
+    <row r="6" ht="13.8" customHeight="1" s="4">
+      <c r="B6" s="3" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentOddEven="0" differentFirst="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;KffffffPage &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>